<commit_message>
integrated read_batch and simulate_synthetic functions
</commit_message>
<xml_diff>
--- a/Sandbox/Raw Data - 02052024/Measurement_09_02_16electrodes_Xusha.xlsx
+++ b/Sandbox/Raw Data - 02052024/Measurement_09_02_16electrodes_Xusha.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>OpenBCISession_2024-02-09_11-10-01</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Покой</t>
   </si>
   <si>
+    <t>Rest</t>
+  </si>
+  <si>
     <t>11-15-45</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
     <t>постоянное легкое моргание</t>
   </si>
   <si>
+    <t>Continuous light blinking</t>
+  </si>
+  <si>
     <t>11-21-20</t>
   </si>
   <si>
@@ -58,6 +64,9 @@
     <t>постоянное сильное моргание</t>
   </si>
   <si>
+    <t>Continuous strong blinking</t>
+  </si>
+  <si>
     <t>11-24-22</t>
   </si>
   <si>
@@ -76,6 +85,9 @@
     <t>постоянное сжимание челюсти</t>
   </si>
   <si>
+    <t>Continuous jaw clenching</t>
+  </si>
+  <si>
     <t>11-28-29</t>
   </si>
   <si>
@@ -94,22 +106,34 @@
     <t>покой с морганием слабым</t>
   </si>
   <si>
+    <t>Rest with weak blinking</t>
+  </si>
+  <si>
     <t>11-32-29</t>
   </si>
   <si>
     <t>покой с морганием сильным</t>
   </si>
   <si>
+    <t>Rest with strong blinking</t>
+  </si>
+  <si>
     <t>11-32-56</t>
   </si>
   <si>
     <t>покой с сжиманием челюсти</t>
   </si>
   <si>
+    <t>Rest with jaw clenching</t>
+  </si>
+  <si>
     <t>11-33-26</t>
   </si>
   <si>
     <t>покой со всем вместе</t>
+  </si>
+  <si>
+    <t>Rest with all together</t>
   </si>
   <si>
     <t>в самом сморщила лицо, челюсть клац и моргнула одновременно</t>
@@ -183,7 +207,7 @@
     <xdr:ext cx="10134600" cy="5572125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -211,7 +235,7 @@
     <xdr:ext cx="12877800" cy="7315200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -437,6 +461,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="33.88"/>
+    <col customWidth="1" min="3" max="3" width="30.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -451,192 +476,264 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>14</v>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>20</v>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>